<commit_message>
On Screen Actions - Full test to verify input data works. But as you can see the test fails because of save window. Let's assume this a new feature and we have 100s of tests. Good thing we created a utility for closing the app because now we just need to update one spot to make them all work
</commit_message>
<xml_diff>
--- a/Utilities/NOV_DevData.xlsx
+++ b/Utilities/NOV_DevData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>id</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Rocks</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
     <t>Is Awesome</t>
   </si>
   <si>
@@ -76,6 +70,9 @@
   </si>
   <si>
     <t>last_Name</t>
+  </si>
+  <si>
+    <t>TestComplete</t>
   </si>
 </sst>
 </file>
@@ -417,7 +414,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,13 +429,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
         <v>1</v>
@@ -452,7 +449,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -464,7 +461,7 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -472,7 +469,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -484,7 +481,7 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -492,19 +489,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
On Screen Actions - Fixing some of the logging and other issues. Also, new version of our application
</commit_message>
<xml_diff>
--- a/Utilities/NOV_DevData.xlsx
+++ b/Utilities/NOV_DevData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>TestComplete</t>
+  </si>
+  <si>
+    <t>product</t>
   </si>
 </sst>
 </file>
@@ -414,7 +417,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B2" sqref="B2:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +492,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Verifications - Adding more but not having to edit individual tests
</commit_message>
<xml_diff>
--- a/Utilities/NOV_DevData.xlsx
+++ b/Utilities/NOV_DevData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>id</t>
   </si>
@@ -76,6 +76,12 @@
   </si>
   <si>
     <t>product</t>
+  </si>
+  <si>
+    <t>newMessage</t>
+  </si>
+  <si>
+    <t>new</t>
   </si>
 </sst>
 </file>
@@ -414,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+      <selection activeCell="G1" sqref="G1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,9 +431,10 @@
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,8 +453,11 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -466,8 +476,11 @@
       <c r="F2" t="s">
         <v>10</v>
       </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -486,8 +499,11 @@
       <c r="F3" t="s">
         <v>11</v>
       </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -502,6 +518,9 @@
       </c>
       <c r="F4" t="s">
         <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>